<commit_message>
Change map sensor to MPXH6400AC6U
</commit_message>
<xml_diff>
--- a/m50-m40-m60_Pnp/Rev 2.2/BOM-speeduino v0.4.3 compatible PCB for m40 rev2.2.xlsx
+++ b/m50-m40-m60_Pnp/Rev 2.2/BOM-speeduino v0.4.3 compatible PCB for m40 rev2.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 2.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50-m40-m60_Pnp\Rev 2.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56714E85-C833-4319-8174-F8AF36B2A268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F815B20-A519-4512-98F8-C5D7B81E5867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="735" windowWidth="28650" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14265" yWindow="3840" windowWidth="31590" windowHeight="16860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H44" authorId="0" shapeId="0" xr:uid="{2B0A136D-4BD2-48D6-8AFA-04F734AF97EE}">
+    <comment ref="H44" authorId="0" shapeId="0" xr:uid="{362156A8-B4EB-4056-A300-76B7EC2E37C4}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-As 4bar map sensor, use MPX4400AP</t>
+As 4bar map sensor, use MPX4400AP
+There is also option to use SOP (MPXA4250AC6U) and SSOP (MPXH6250AC6U) package ones.
+SSOP 4bar version is: MPXH6400AC6U </t>
         </r>
       </text>
     </comment>
@@ -142,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="296">
   <si>
     <t>Value</t>
   </si>
@@ -354,18 +356,6 @@
     <t>5mm-LED</t>
   </si>
   <si>
-    <t>MPX4250AP-ND</t>
-  </si>
-  <si>
-    <t>6-SIP</t>
-  </si>
-  <si>
-    <t>SENSOR ABS PRESS 36.3 PSI MAX</t>
-  </si>
-  <si>
-    <t>MPX4250A</t>
-  </si>
-  <si>
     <t>Male pins</t>
   </si>
   <si>
@@ -531,12 +521,6 @@
     <t>Mouser Price (USD)</t>
   </si>
   <si>
-    <t>MPX4250AP</t>
-  </si>
-  <si>
-    <t>841-MPX4250AP</t>
-  </si>
-  <si>
     <t>579-TC4424EPA</t>
   </si>
   <si>
@@ -661,9 +645,6 @@
   </si>
   <si>
     <t>603-FMF-25FTF52100K</t>
-  </si>
-  <si>
-    <t>2.5-Bar MAP sensor</t>
   </si>
   <si>
     <t>7.5k</t>
@@ -1245,6 +1226,24 @@
   </si>
   <si>
     <t>C1,C3,C5,C7,C9,C13,C15,C21,C22,C29</t>
+  </si>
+  <si>
+    <t>MPXH6400AC6U</t>
+  </si>
+  <si>
+    <t>4-Bar MAP sensor</t>
+  </si>
+  <si>
+    <t>SENSOR ABS PRESS 58 PSI MAX</t>
+  </si>
+  <si>
+    <t>SSOP-8</t>
+  </si>
+  <si>
+    <t>MPXH6400AC6U-ND</t>
+  </si>
+  <si>
+    <t>841-MPXH6400AC6U</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1477,6 +1476,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1534,7 +1548,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1585,13 +1599,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1612,7 +1623,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1621,7 +1632,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1635,6 +1646,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2033,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2055,10 +2075,10 @@
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2070,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -2082,31 +2102,31 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1">
@@ -2146,7 +2166,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -2156,13 +2176,13 @@
         <v>12</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K3" s="5">
         <v>1.7</v>
@@ -2202,13 +2222,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
@@ -2218,13 +2238,13 @@
         <v>12</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="K4" s="5">
         <v>0.66</v>
@@ -2264,13 +2284,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
@@ -2280,13 +2300,13 @@
         <v>12</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K5" s="5">
         <v>0.32</v>
@@ -2332,7 +2352,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
@@ -2342,13 +2362,13 @@
         <v>12</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="K6" s="5">
         <v>1.57</v>
@@ -2388,13 +2408,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -2404,13 +2424,13 @@
         <v>9</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K7" s="5">
         <v>0.62</v>
@@ -2450,13 +2470,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
@@ -2466,13 +2486,13 @@
         <v>12</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="K8" s="5">
         <v>0.24</v>
@@ -2512,13 +2532,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>11</v>
@@ -2528,13 +2548,13 @@
         <v>12</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K9" s="5">
         <v>0.66</v>
@@ -2574,13 +2594,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -2590,13 +2610,13 @@
         <v>9</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>252</v>
+        <v>246</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>245</v>
       </c>
       <c r="K10" s="5">
         <v>0.3</v>
@@ -2636,13 +2656,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>11</v>
@@ -2652,13 +2672,13 @@
         <v>12</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K11" s="5">
         <v>0.25</v>
@@ -2727,10 +2747,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>18</v>
@@ -2749,7 +2769,7 @@
         <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K13" s="5">
         <v>0.34</v>
@@ -2789,10 +2809,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2811,7 +2831,7 @@
         <v>26</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K14" s="5">
         <v>0.39</v>
@@ -2851,13 +2871,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>69</v>
@@ -2865,13 +2885,13 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K15" s="5">
         <v>0.47</v>
@@ -2911,7 +2931,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
@@ -2933,7 +2953,7 @@
         <v>31</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K16" s="5">
         <v>0.11</v>
@@ -3005,7 +3025,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>32</v>
@@ -3027,7 +3047,7 @@
         <v>37</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K18" s="5">
         <v>0.72</v>
@@ -3099,32 +3119,32 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K20" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="21">
         <v>2.95</v>
       </c>
       <c r="M20" s="6">
@@ -3136,7 +3156,7 @@
         <v>11.8</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="P20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3160,32 +3180,32 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>288</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>289</v>
+        <v>178</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>282</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="K21" s="6">
         <v>1</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="23">
         <v>0.88200000000000001</v>
       </c>
       <c r="M21" s="6">
@@ -3219,32 +3239,32 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="I22" s="26" t="s">
-        <v>204</v>
+        <v>191</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>197</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="K22" s="6">
         <v>0.38</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="23">
         <v>0.76</v>
       </c>
       <c r="M22" s="6">
@@ -3278,32 +3298,32 @@
         <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="I23" s="26" t="s">
-        <v>202</v>
+        <v>191</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>195</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K23" s="6">
         <v>0.23</v>
       </c>
-      <c r="L23" s="24">
+      <c r="L23" s="23">
         <v>0.49</v>
       </c>
       <c r="M23" s="6">
@@ -3371,13 +3391,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>61</v>
@@ -3387,13 +3407,13 @@
         <v>38</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K25" s="6">
         <v>1.51</v>
@@ -3433,29 +3453,29 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>191</v>
+        <v>174</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>184</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="K26" s="6">
         <v>2.62</v>
@@ -3495,30 +3515,30 @@
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>230</v>
+      <c r="B27" s="27" t="s">
+        <v>223</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>235</v>
+        <v>226</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>228</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K27" s="6">
         <v>0.25</v>
@@ -3558,29 +3578,29 @@
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="I28" s="26" t="s">
-        <v>192</v>
+        <v>182</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>185</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="K28" s="6">
         <v>0.25</v>
@@ -3635,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>39</v>
@@ -3649,13 +3669,13 @@
         <v>41</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>42</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="K30" s="5">
         <v>0.08</v>
@@ -3691,8 +3711,8 @@
     </row>
     <row r="31" spans="1:19" ht="26.25" thickBot="1">
       <c r="A31" s="17"/>
-      <c r="B31" s="31" t="s">
-        <v>269</v>
+      <c r="B31" s="30" t="s">
+        <v>262</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3715,7 +3735,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>43</v>
@@ -3729,13 +3749,13 @@
         <v>41</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K32" s="5">
         <v>0.06</v>
@@ -3775,27 +3795,27 @@
         <v>2</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C33" s="12">
         <v>680</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="K33" s="13">
         <v>0.22</v>
@@ -3812,7 +3832,7 @@
         <v>0.3</v>
       </c>
       <c r="O33" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P33" s="4" t="str">
         <f t="shared" si="10"/>
@@ -3837,7 +3857,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C34" s="3">
         <v>470</v>
@@ -3857,7 +3877,7 @@
         <v>49</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K34" s="5">
         <v>0.11</v>
@@ -3897,13 +3917,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>50</v>
@@ -3913,13 +3933,13 @@
         <v>41</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="K35" s="5">
         <v>0.14000000000000001</v>
@@ -3959,10 +3979,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>51</v>
@@ -3979,7 +3999,7 @@
         <v>53</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K36" s="5">
         <v>0.46</v>
@@ -3996,7 +4016,7 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P36" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4021,7 +4041,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>54</v>
@@ -4035,13 +4055,13 @@
         <v>41</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K37" s="5">
         <v>0.1</v>
@@ -4081,27 +4101,27 @@
         <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C38" s="3">
         <v>150</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="K38" s="5">
         <v>0.27</v>
@@ -4141,13 +4161,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -4155,13 +4175,13 @@
         <v>41</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5">
@@ -4251,7 +4271,7 @@
         <v>59</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K41" s="5">
         <v>1.68</v>
@@ -4291,29 +4311,29 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>240</v>
+        <v>230</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>233</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="K42" s="5">
         <v>0.59</v>
@@ -4329,16 +4349,16 @@
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="Q42" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="R42" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="S42" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="26.25" thickBot="1">
@@ -4346,30 +4366,30 @@
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="B43" s="21" t="s">
-        <v>216</v>
+      <c r="B43" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="I43" s="27" t="s">
-        <v>214</v>
+        <v>206</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K43" s="6">
         <v>12.79</v>
@@ -4409,29 +4429,29 @@
         <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>73</v>
+        <v>290</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>72</v>
+        <v>292</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>71</v>
+        <v>293</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>130</v>
+      <c r="H44" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="I44" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>295</v>
       </c>
       <c r="K44" s="6">
         <v>15.41</v>
@@ -4440,29 +4460,29 @@
         <v>15.37</v>
       </c>
       <c r="M44" s="6">
-        <f>K44*A44</f>
+        <f t="shared" ref="M44" si="19">K44*A44</f>
         <v>15.41</v>
       </c>
       <c r="N44" s="6">
-        <f>L44*A44</f>
+        <f t="shared" ref="N44" si="20">L44*A44</f>
         <v>15.37</v>
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>1,MPX4250AP-ND</v>
+        <v>1,MPXH6400AC6U-ND</v>
       </c>
       <c r="Q44" t="str">
         <f>A44&amp;"x "&amp;C44</f>
-        <v>1x 2.5-Bar MAP sensor</v>
+        <v>1x 4-Bar MAP sensor</v>
       </c>
       <c r="R44" t="str">
         <f t="shared" si="18"/>
-        <v>841-MPX4250AP|1</v>
+        <v>841-MPXH6400AC6U|1</v>
       </c>
       <c r="S44" t="str">
         <f>H44&amp;" "&amp;A44</f>
-        <v>MPX4250AP 1</v>
+        <v>MPXH6400AC6U 1</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="26.25" thickBot="1">
@@ -4471,29 +4491,29 @@
         <v>2</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12" t="s">
         <v>63</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K45" s="19">
         <v>2.92</v>
@@ -4533,29 +4553,29 @@
         <v>1</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="K46" s="6">
         <v>2.4</v>
@@ -4595,29 +4615,29 @@
         <v>2</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="K47" s="6">
         <v>1.41</v>
@@ -4679,7 +4699,7 @@
     <row r="49" spans="1:19" ht="16.5" thickBot="1">
       <c r="A49" s="15"/>
       <c r="B49" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -4708,16 +4728,16 @@
         <v>1</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -4736,27 +4756,27 @@
         <v>1</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K51" s="6">
         <v>0.33</v>
@@ -4795,27 +4815,27 @@
         <v>17</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="K52" s="6">
         <v>0.16</v>
@@ -4873,13 +4893,13 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="20"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="33" t="s">
+      <c r="H54" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="I54" s="34"/>
-      <c r="J54" s="29"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="28"/>
       <c r="K54" s="1" t="s">
         <v>64</v>
       </c>
@@ -4898,22 +4918,22 @@
     </row>
     <row r="58" spans="1:19">
       <c r="B58" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:19">
       <c r="B59" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:19">
       <c r="B60" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:19">
       <c r="B61" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4928,14 +4948,13 @@
     <hyperlink ref="I30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="I35" r:id="rId5" display="985-1047-1-ND" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="I36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I44" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I3" r:id="rId8" display="478-1842-ND" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I7" r:id="rId9" display="445-5312-ND" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I8" r:id="rId10" display="399-4148-ND" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I3" r:id="rId7" display="478-1842-ND" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I7" r:id="rId8" display="445-5312-ND" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I8" r:id="rId9" display="399-4148-ND" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="31" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <pageSetup paperSize="9" scale="31" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>